<commit_message>
added battery and button
</commit_message>
<xml_diff>
--- a/Component Links/Component Links.xlsx
+++ b/Component Links/Component Links.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pinger-V2\Component Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73422F58-7420-4888-9194-1BE1B8621494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0CC972-C6AC-4529-863D-61747104FE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{0F8150A8-AA68-4604-9B98-D599FD82A279}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0F8150A8-AA68-4604-9B98-D599FD82A279}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Component</t>
   </si>
@@ -42,6 +42,21 @@
   </si>
   <si>
     <t>Mech/Elec/Firm</t>
+  </si>
+  <si>
+    <t>Elec</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>https://www.18650batterystore.com/en-ca/products/ydl-14500-battery</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adam-tech/SW-PB2-2EZ-A-RR-3-L1/15284423</t>
   </si>
 </sst>
 </file>
@@ -393,19 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B05EED-111F-434E-A5EF-BF1534CF173A}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,6 +430,28 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added buck/boost and boost
</commit_message>
<xml_diff>
--- a/Component Links/Component Links.xlsx
+++ b/Component Links/Component Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pinger-V2\Component Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD8ED4C-8604-4E40-A46D-8EA73D131B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D301FE-5AF6-43C4-B55E-331B01D3CA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0F8150A8-AA68-4604-9B98-D599FD82A279}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Component</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Mech/Elec</t>
+  </si>
+  <si>
+    <t>Buck Boost</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/TPS55340RTER/3503781</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/TPS630702RNMR/10434765</t>
   </si>
 </sst>
 </file>
@@ -437,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B05EED-111F-434E-A5EF-BF1534CF173A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,6 +517,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CED35EAF-B3AE-47B3-AB6C-59F0F160F593}"/>

</xml_diff>

<commit_message>
added components and finished buck/boost
</commit_message>
<xml_diff>
--- a/Component Links/Component Links.xlsx
+++ b/Component Links/Component Links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimiy\repos\PingerProject\Component Links\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pinger-V2\Component Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649D941C-AFFE-4685-AB9E-D98947721F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E53E95B-04F5-4657-A957-79CE721CA360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{0F8150A8-AA68-4604-9B98-D599FD82A279}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F8150A8-AA68-4604-9B98-D599FD82A279}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Component</t>
   </si>
@@ -93,6 +93,24 @@
   </si>
   <si>
     <t>https://www.mouser.ca/datasheet/2/277/MP2759AGQ-2888162.pdf</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/pui-audio-inc/AS03608AS-R/9863635</t>
+  </si>
+  <si>
+    <t>Audio Amp</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/1552/5353653</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/1712/5629429</t>
   </si>
 </sst>
 </file>
@@ -455,20 +473,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B05EED-111F-434E-A5EF-BF1534CF173A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="61.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -490,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -501,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -512,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -523,7 +541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -534,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -545,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -553,6 +571,39 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>